<commit_message>
prediction added to excel
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,50 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2BDD9F-5D82-49C3-BE32-76CD89DFAA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="test" state="visible" r:id="rId4"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Address</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Bedrooms</t>
+  </si>
+  <si>
+    <t>Badrooms</t>
+  </si>
+  <si>
+    <t>Total size</t>
   </si>
   <si>
     <t>Price</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Bedrooms</t>
-  </si>
-  <si>
-    <t>Bathrooms</t>
-  </si>
-  <si>
-    <t>Total Size</t>
+    <t>Predicted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -408,11 +424,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F223"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H223"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -445,8 +466,22 @@
       <c r="D2">
         <v>62.69</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>504900</v>
+      </c>
+      <c r="F2">
+        <v>547896.43000000005</v>
+      </c>
+      <c r="G2">
+        <f>ABS(E2-F2)</f>
+        <v>42996.430000000051</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(G2:G223)</f>
+        <v>90436.160000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -459,8 +494,18 @@
       <c r="D3">
         <v>93.67</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>505900</v>
+      </c>
+      <c r="F3">
+        <v>689838.33</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="0">ABS(E3-F3)</f>
+        <v>183938.32999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -471,10 +516,20 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>39.63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39.630000000000003</v>
+      </c>
+      <c r="E4">
+        <v>508000</v>
+      </c>
+      <c r="F4">
+        <v>428196.61</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>79803.390000000014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -487,8 +542,18 @@
       <c r="D5">
         <v>54.87</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>508800</v>
+      </c>
+      <c r="F5">
+        <v>508114.67</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>685.3300000000163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -501,8 +566,18 @@
       <c r="D6">
         <v>88.19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>509000</v>
+      </c>
+      <c r="F6">
+        <v>668244.26</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>159244.26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -515,8 +590,18 @@
       <c r="D7">
         <v>57.31</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>509000</v>
+      </c>
+      <c r="F7">
+        <v>497865.08</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>11134.919999999984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -529,8 +614,18 @@
       <c r="D8">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>509000</v>
+      </c>
+      <c r="F8">
+        <v>496643.52</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>12356.479999999981</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -543,8 +638,18 @@
       <c r="D9">
         <v>55.66</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>509900</v>
+      </c>
+      <c r="F9">
+        <v>511227.68</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1327.679999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -557,8 +662,18 @@
       <c r="D10">
         <v>83.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>509900</v>
+      </c>
+      <c r="F10">
+        <v>648186.99</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>138286.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -571,8 +686,18 @@
       <c r="D11">
         <v>83.56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>509900</v>
+      </c>
+      <c r="F11">
+        <v>649999.63</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>140099.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -585,8 +710,18 @@
       <c r="D12">
         <v>87.41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>509990</v>
+      </c>
+      <c r="F12">
+        <v>665170.65</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>155180.65000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -599,8 +734,18 @@
       <c r="D13">
         <v>60.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>509990</v>
+      </c>
+      <c r="F13">
+        <v>559919.25</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>49929.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -613,8 +758,18 @@
       <c r="D14">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>510000</v>
+      </c>
+      <c r="F14">
+        <v>453459.6</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>56540.400000000023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -627,8 +782,18 @@
       <c r="D15">
         <v>56.72</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>510000</v>
+      </c>
+      <c r="F15">
+        <v>495540.17</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>14459.830000000016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -641,8 +806,18 @@
       <c r="D16">
         <v>57.37</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>513000</v>
+      </c>
+      <c r="F16">
+        <v>517965.98</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>4965.9799999999814</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -655,8 +830,18 @@
       <c r="D17">
         <v>67.48</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>514900</v>
+      </c>
+      <c r="F17">
+        <v>586636.01</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>71736.010000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -669,8 +854,18 @@
       <c r="D18">
         <v>96.82</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>514900</v>
+      </c>
+      <c r="F18">
+        <v>702250.98</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>187350.97999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -683,8 +878,18 @@
       <c r="D19">
         <v>61.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>515000</v>
+      </c>
+      <c r="F19">
+        <v>532388.30000000005</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>17388.300000000047</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -697,8 +902,18 @@
       <c r="D20">
         <v>92.57</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>515000</v>
+      </c>
+      <c r="F20">
+        <v>685503.76</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>170503.76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -711,8 +926,18 @@
       <c r="D21">
         <v>88.85</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>515000</v>
+      </c>
+      <c r="F21">
+        <v>670845.01</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>155845.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -725,8 +950,18 @@
       <c r="D22">
         <v>57.29</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>515000</v>
+      </c>
+      <c r="F22">
+        <v>517650.74</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>2650.7399999999907</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -737,10 +972,20 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>75.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="E23">
+        <v>515000</v>
+      </c>
+      <c r="F23">
+        <v>587831.47</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>72831.469999999972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -753,8 +998,18 @@
       <c r="D24">
         <v>56.76</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>516000</v>
+      </c>
+      <c r="F24">
+        <v>524529.12</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>8529.1199999999953</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -767,8 +1022,18 @@
       <c r="D25">
         <v>73.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>518888</v>
+      </c>
+      <c r="F25">
+        <v>581526.63</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>62638.630000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -781,8 +1046,18 @@
       <c r="D26">
         <v>63.45</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>518888</v>
+      </c>
+      <c r="F26">
+        <v>541924.36</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>23036.359999999986</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -793,10 +1068,20 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>77.32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.319999999999993</v>
+      </c>
+      <c r="E27">
+        <v>518900</v>
+      </c>
+      <c r="F27">
+        <v>625410.76</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>106510.76000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -809,8 +1094,18 @@
       <c r="D28">
         <v>64.03</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>519000</v>
+      </c>
+      <c r="F28">
+        <v>553176.73</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>34176.729999999981</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -823,8 +1118,18 @@
       <c r="D29">
         <v>57.96</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>519000</v>
+      </c>
+      <c r="F29">
+        <v>529257.75</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>10257.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -837,8 +1142,18 @@
       <c r="D30">
         <v>54.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>519700</v>
+      </c>
+      <c r="F30">
+        <v>537064.21</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>17364.209999999963</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -851,8 +1166,18 @@
       <c r="D31">
         <v>63.24</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>519900</v>
+      </c>
+      <c r="F31">
+        <v>541096.85</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>21196.849999999977</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -865,8 +1190,18 @@
       <c r="D32">
         <v>56.24</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>519900</v>
+      </c>
+      <c r="F32">
+        <v>513513.19</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>6386.8099999999977</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -879,8 +1214,18 @@
       <c r="D33">
         <v>59.83</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>519900</v>
+      </c>
+      <c r="F33">
+        <v>536626.53</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>16726.530000000028</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -893,8 +1238,18 @@
       <c r="D34">
         <v>60.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>519900</v>
+      </c>
+      <c r="F34">
+        <v>560707.36</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>40807.359999999986</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -907,8 +1262,18 @@
       <c r="D35">
         <v>76.38</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>519900</v>
+      </c>
+      <c r="F35">
+        <v>601842.19999999995</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>81942.199999999953</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
@@ -921,8 +1286,18 @@
       <c r="D36">
         <v>61.14</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>520000</v>
+      </c>
+      <c r="F36">
+        <v>532821.75</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>12821.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1</v>
       </c>
@@ -935,8 +1310,18 @@
       <c r="D37">
         <v>54.78</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>520000</v>
+      </c>
+      <c r="F37">
+        <v>507760.02</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>12239.979999999981</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
@@ -949,8 +1334,18 @@
       <c r="D38">
         <v>34.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>520000</v>
+      </c>
+      <c r="F38">
+        <v>426861.06</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>93138.94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1</v>
       </c>
@@ -963,8 +1358,18 @@
       <c r="D39">
         <v>43.27</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>520000</v>
+      </c>
+      <c r="F39">
+        <v>442540.12</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>77459.88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -977,8 +1382,18 @@
       <c r="D40">
         <v>44.69</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>521999</v>
+      </c>
+      <c r="F40">
+        <v>457102.53</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>64896.469999999972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1</v>
       </c>
@@ -991,8 +1406,18 @@
       <c r="D41">
         <v>72.25</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>524000</v>
+      </c>
+      <c r="F41">
+        <v>585567.84</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>61567.839999999967</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1005,8 +1430,18 @@
       <c r="D42">
         <v>83.1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>524900</v>
+      </c>
+      <c r="F42">
+        <v>648186.99</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>123286.98999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1019,8 +1454,18 @@
       <c r="D43">
         <v>55.79</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>524900</v>
+      </c>
+      <c r="F43">
+        <v>520706.81</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>4193.1900000000023</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1033,8 +1478,18 @@
       <c r="D44">
         <v>53.27</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>524999</v>
+      </c>
+      <c r="F44">
+        <v>501809.83</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>23189.169999999984</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1047,8 +1502,18 @@
       <c r="D45">
         <v>54.56</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>525000</v>
+      </c>
+      <c r="F45">
+        <v>506893.11</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>18106.890000000014</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1061,8 +1526,18 @@
       <c r="D46">
         <v>58.69</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>525000</v>
+      </c>
+      <c r="F46">
+        <v>523167.47</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>1832.5300000000279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1075,8 +1550,18 @@
       <c r="D47">
         <v>56.97</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>525000</v>
+      </c>
+      <c r="F47">
+        <v>516389.77</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>8610.2299999999814</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1089,8 +1574,18 @@
       <c r="D48">
         <v>79.14</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>525000</v>
+      </c>
+      <c r="F48">
+        <v>632582.52</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>107582.52000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1103,8 +1598,18 @@
       <c r="D49">
         <v>60.53</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>528800</v>
+      </c>
+      <c r="F49">
+        <v>539384.9</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>10584.900000000023</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1117,8 +1622,18 @@
       <c r="D50">
         <v>65.55</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>529900</v>
+      </c>
+      <c r="F50">
+        <v>530335</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -1131,8 +1646,18 @@
       <c r="D51">
         <v>50.75</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>529900</v>
+      </c>
+      <c r="F51">
+        <v>491879.71</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>38020.289999999979</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1145,8 +1670,18 @@
       <c r="D52">
         <v>59.37</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>529900</v>
+      </c>
+      <c r="F52">
+        <v>525847.03</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>4052.9699999999721</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1159,8 +1694,18 @@
       <c r="D53">
         <v>65.78</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>530000</v>
+      </c>
+      <c r="F53">
+        <v>560072.65</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>30072.650000000023</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1173,8 +1718,18 @@
       <c r="D54">
         <v>70.12</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>530000</v>
+      </c>
+      <c r="F54">
+        <v>577174.52</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>47174.520000000019</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1</v>
       </c>
@@ -1187,8 +1742,18 @@
       <c r="D55">
         <v>49.45</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>532000</v>
+      </c>
+      <c r="F55">
+        <v>495723.89</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>36276.109999999986</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1201,8 +1766,18 @@
       <c r="D56">
         <v>56.78</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>534000</v>
+      </c>
+      <c r="F56">
+        <v>524607.93000000005</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>9392.0699999999488</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1</v>
       </c>
@@ -1215,8 +1790,18 @@
       <c r="D57">
         <v>72.13</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>534900</v>
+      </c>
+      <c r="F57">
+        <v>576128.11</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>41228.109999999986</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1229,8 +1814,18 @@
       <c r="D58">
         <v>84.49</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>535000</v>
+      </c>
+      <c r="F58">
+        <v>633799.85</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>98799.849999999977</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1243,8 +1838,18 @@
       <c r="D59">
         <v>46.59</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>535900</v>
+      </c>
+      <c r="F59">
+        <v>475487.13</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>60412.869999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1</v>
       </c>
@@ -1257,8 +1862,18 @@
       <c r="D60">
         <v>57.6</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>538900</v>
+      </c>
+      <c r="F60">
+        <v>527839.16</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>11060.839999999967</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1</v>
       </c>
@@ -1271,8 +1886,18 @@
       <c r="D61">
         <v>52.34</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>539000</v>
+      </c>
+      <c r="F61">
+        <v>498145.14</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>40854.859999999986</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1</v>
       </c>
@@ -1283,10 +1908,20 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>71.35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="E62">
+        <v>539000</v>
+      </c>
+      <c r="F62">
+        <v>601885.84</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>62885.839999999967</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1299,8 +1934,18 @@
       <c r="D63">
         <v>73.87</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>539000</v>
+      </c>
+      <c r="F63">
+        <v>602849.09</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>63849.089999999967</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1</v>
       </c>
@@ -1313,8 +1958,18 @@
       <c r="D64">
         <v>85.07</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>539000</v>
+      </c>
+      <c r="F64">
+        <v>655949.82999999996</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>116949.82999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1</v>
       </c>
@@ -1327,8 +1982,18 @@
       <c r="D65">
         <v>51.3</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>539000</v>
+      </c>
+      <c r="F65">
+        <v>503013.86</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>35986.140000000014</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1</v>
       </c>
@@ -1341,8 +2006,18 @@
       <c r="D66">
         <v>55.01</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>539500</v>
+      </c>
+      <c r="F66">
+        <v>508666.34</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>30833.659999999974</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1</v>
       </c>
@@ -1355,8 +2030,18 @@
       <c r="D67">
         <v>72.27</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>539800</v>
+      </c>
+      <c r="F67">
+        <v>605511.12</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G130" si="1">ABS(E67-F67)</f>
+        <v>65711.12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1</v>
       </c>
@@ -1369,8 +2054,18 @@
       <c r="D68">
         <v>49.97</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>539888</v>
+      </c>
+      <c r="F68">
+        <v>497772.96</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="1"/>
+        <v>42115.039999999979</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1</v>
       </c>
@@ -1383,8 +2078,18 @@
       <c r="D69">
         <v>61.49</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>539900</v>
+      </c>
+      <c r="F69">
+        <v>534200.93999999994</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="1"/>
+        <v>5699.0600000000559</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
@@ -1397,8 +2102,18 @@
       <c r="D70">
         <v>57.85</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>539900</v>
+      </c>
+      <c r="F70">
+        <v>528824.29</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="1"/>
+        <v>11075.709999999963</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1</v>
       </c>
@@ -1411,8 +2126,18 @@
       <c r="D71">
         <v>60.67</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>539900</v>
+      </c>
+      <c r="F71">
+        <v>539936.56999999995</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="1"/>
+        <v>36.569999999948777</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1</v>
       </c>
@@ -1425,8 +2150,18 @@
       <c r="D72">
         <v>64.02</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>540000</v>
+      </c>
+      <c r="F72">
+        <v>553137.32999999996</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="1"/>
+        <v>13137.329999999958</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1</v>
       </c>
@@ -1439,8 +2174,18 @@
       <c r="D73">
         <v>85.8</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>544900</v>
+      </c>
+      <c r="F73">
+        <v>658826.41</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="1"/>
+        <v>113926.41000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1</v>
       </c>
@@ -1453,8 +2198,18 @@
       <c r="D74">
         <v>53.78</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>544900</v>
+      </c>
+      <c r="F74">
+        <v>483955.03</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="1"/>
+        <v>60944.969999999972</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1465,10 +2220,20 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <v>68.49</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68.489999999999995</v>
+      </c>
+      <c r="E75">
+        <v>545000</v>
+      </c>
+      <c r="F75">
+        <v>581649.06999999995</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="1"/>
+        <v>36649.069999999949</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1</v>
       </c>
@@ -1481,8 +2246,18 @@
       <c r="D76">
         <v>57.34</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>548000</v>
+      </c>
+      <c r="F76">
+        <v>517847.76</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="1"/>
+        <v>30152.239999999991</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1</v>
       </c>
@@ -1495,8 +2270,18 @@
       <c r="D77">
         <v>97.53</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>549000</v>
+      </c>
+      <c r="F77">
+        <v>705048.76</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="1"/>
+        <v>156048.76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1</v>
       </c>
@@ -1509,8 +2294,18 @@
       <c r="D78">
         <v>38.81</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>549000</v>
+      </c>
+      <c r="F78">
+        <v>444829.85</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="1"/>
+        <v>104170.15000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1</v>
       </c>
@@ -1523,8 +2318,18 @@
       <c r="D79">
         <v>69.89</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>549000</v>
+      </c>
+      <c r="F79">
+        <v>576268.19999999995</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="1"/>
+        <v>27268.199999999953</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1</v>
       </c>
@@ -1537,8 +2342,18 @@
       <c r="D80">
         <v>57.94</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>549000</v>
+      </c>
+      <c r="F80">
+        <v>520212.08</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="1"/>
+        <v>28787.919999999984</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1</v>
       </c>
@@ -1551,8 +2366,18 @@
       <c r="D81">
         <v>71.55</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>549000</v>
+      </c>
+      <c r="F81">
+        <v>573842.61</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="1"/>
+        <v>24842.609999999986</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1</v>
       </c>
@@ -1565,8 +2390,18 @@
       <c r="D82">
         <v>57.78</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>549900</v>
+      </c>
+      <c r="F82">
+        <v>508683.99</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="1"/>
+        <v>41216.010000000009</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1</v>
       </c>
@@ -1579,8 +2414,18 @@
       <c r="D83">
         <v>59.1</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>549900</v>
+      </c>
+      <c r="F83">
+        <v>533749.94999999995</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="1"/>
+        <v>16150.050000000047</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1</v>
       </c>
@@ -1593,8 +2438,18 @@
       <c r="D84">
         <v>87.73</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>549900</v>
+      </c>
+      <c r="F84">
+        <v>666431.62</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="1"/>
+        <v>116531.62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1</v>
       </c>
@@ -1607,8 +2462,18 @@
       <c r="D85">
         <v>87</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>549900</v>
+      </c>
+      <c r="F85">
+        <v>663555.04</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="1"/>
+        <v>113655.04000000004</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1</v>
       </c>
@@ -1621,8 +2486,18 @@
       <c r="D86">
         <v>58.14</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>549900</v>
+      </c>
+      <c r="F86">
+        <v>529967.04</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="1"/>
+        <v>19932.959999999963</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>1</v>
       </c>
@@ -1635,8 +2510,18 @@
       <c r="D87">
         <v>77.84</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>549900</v>
+      </c>
+      <c r="F87">
+        <v>627459.83999999997</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="1"/>
+        <v>77559.839999999967</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1</v>
       </c>
@@ -1649,8 +2534,18 @@
       <c r="D88">
         <v>41.63</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>550000</v>
+      </c>
+      <c r="F88">
+        <v>464908.99</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="1"/>
+        <v>85091.010000000009</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>1</v>
       </c>
@@ -1663,8 +2558,18 @@
       <c r="D89">
         <v>46.73</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>552800</v>
+      </c>
+      <c r="F89">
+        <v>476038.8</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="1"/>
+        <v>76761.200000000012</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>1</v>
       </c>
@@ -1677,8 +2582,18 @@
       <c r="D90">
         <v>65.19</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>554988</v>
+      </c>
+      <c r="F90">
+        <v>577612.21</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="1"/>
+        <v>22624.209999999963</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1</v>
       </c>
@@ -1691,8 +2606,18 @@
       <c r="D91">
         <v>109.96</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>555000</v>
+      </c>
+      <c r="F91">
+        <v>745062.61</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="1"/>
+        <v>190062.61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>1</v>
       </c>
@@ -1705,8 +2630,18 @@
       <c r="D92">
         <v>60.45</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>555000</v>
+      </c>
+      <c r="F92">
+        <v>539069.65</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="1"/>
+        <v>15930.349999999977</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>1</v>
       </c>
@@ -1719,8 +2654,18 @@
       <c r="D93">
         <v>53.21</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>555000</v>
+      </c>
+      <c r="F93">
+        <v>510540.26</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="1"/>
+        <v>44459.739999999991</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>1</v>
       </c>
@@ -1733,8 +2678,18 @@
       <c r="D94">
         <v>49.37</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>558800</v>
+      </c>
+      <c r="F94">
+        <v>495408.65</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="1"/>
+        <v>63391.349999999977</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>1</v>
       </c>
@@ -1747,8 +2702,18 @@
       <c r="D95">
         <v>54.54</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>559000</v>
+      </c>
+      <c r="F95">
+        <v>486949.83</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="1"/>
+        <v>72050.169999999984</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1</v>
       </c>
@@ -1761,8 +2726,18 @@
       <c r="D96">
         <v>65.17</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>559000</v>
+      </c>
+      <c r="F96">
+        <v>557668.93000000005</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="1"/>
+        <v>1331.0699999999488</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1</v>
       </c>
@@ -1775,8 +2750,18 @@
       <c r="D97">
         <v>60.15</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>559000</v>
+      </c>
+      <c r="F97">
+        <v>557751.97</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="1"/>
+        <v>1248.0300000000279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1</v>
       </c>
@@ -1789,8 +2774,18 @@
       <c r="D98">
         <v>57.85</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>559900</v>
+      </c>
+      <c r="F98">
+        <v>528824.29</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="1"/>
+        <v>31075.709999999963</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1</v>
       </c>
@@ -1803,8 +2798,18 @@
       <c r="D99">
         <v>60.97</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>559900</v>
+      </c>
+      <c r="F99">
+        <v>560983.18999999994</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="1"/>
+        <v>1083.1899999999441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1</v>
       </c>
@@ -1817,8 +2822,18 @@
       <c r="D100">
         <v>48.27</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>559999</v>
+      </c>
+      <c r="F100">
+        <v>510938.54</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="1"/>
+        <v>49060.460000000021</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1</v>
       </c>
@@ -1831,8 +2846,18 @@
       <c r="D101">
         <v>97.32</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>559999</v>
+      </c>
+      <c r="F101">
+        <v>704221.25</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="1"/>
+        <v>144222.25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1</v>
       </c>
@@ -1845,8 +2870,18 @@
       <c r="D102">
         <v>61.76</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>564900</v>
+      </c>
+      <c r="F102">
+        <v>535264.88</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="1"/>
+        <v>29635.119999999995</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1</v>
       </c>
@@ -1859,8 +2894,18 @@
       <c r="D103">
         <v>61.75</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <v>565000</v>
+      </c>
+      <c r="F103">
+        <v>544192.34</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="1"/>
+        <v>20807.660000000033</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1</v>
       </c>
@@ -1873,8 +2918,18 @@
       <c r="D104">
         <v>92.99</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>565000</v>
+      </c>
+      <c r="F104">
+        <v>667294.31000000006</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="1"/>
+        <v>102294.31000000006</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1</v>
       </c>
@@ -1887,8 +2942,18 @@
       <c r="D105">
         <v>67.27</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>569000</v>
+      </c>
+      <c r="F105">
+        <v>605672.95999999996</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="1"/>
+        <v>36672.959999999963</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1</v>
       </c>
@@ -1901,8 +2966,18 @@
       <c r="D106">
         <v>64.92</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>569800</v>
+      </c>
+      <c r="F106">
+        <v>576548.27</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="1"/>
+        <v>6748.2700000000186</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1</v>
       </c>
@@ -1915,8 +2990,18 @@
       <c r="D107">
         <v>72.47</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <v>569900</v>
+      </c>
+      <c r="F107">
+        <v>566570.29</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="1"/>
+        <v>3329.7099999999627</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1</v>
       </c>
@@ -1929,8 +3014,18 @@
       <c r="D108">
         <v>75.25</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>569900</v>
+      </c>
+      <c r="F108">
+        <v>597389.41</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="1"/>
+        <v>27489.410000000033</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1</v>
       </c>
@@ -1943,8 +3038,18 @@
       <c r="D109">
         <v>59.42</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>569900</v>
+      </c>
+      <c r="F109">
+        <v>526044.05000000005</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="1"/>
+        <v>43855.949999999953</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1</v>
       </c>
@@ -1957,8 +3062,18 @@
       <c r="D110">
         <v>90.43</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <v>569900</v>
+      </c>
+      <c r="F110">
+        <v>657206.56999999995</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="1"/>
+        <v>87306.569999999949</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1</v>
       </c>
@@ -1971,8 +3086,18 @@
       <c r="D111">
         <v>53.97</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111">
+        <v>569900</v>
+      </c>
+      <c r="F111">
+        <v>513535.06</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="1"/>
+        <v>56364.94</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>1</v>
       </c>
@@ -1985,8 +3110,18 @@
       <c r="D112">
         <v>69.97</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <v>574900</v>
+      </c>
+      <c r="F112">
+        <v>576583.43999999994</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="1"/>
+        <v>1683.4399999999441</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>1</v>
       </c>
@@ -1999,8 +3134,18 @@
       <c r="D113">
         <v>61.51</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <v>574900</v>
+      </c>
+      <c r="F113">
+        <v>543246.61</v>
+      </c>
+      <c r="G113">
+        <f t="shared" si="1"/>
+        <v>31653.390000000014</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1</v>
       </c>
@@ -2013,8 +3158,18 @@
       <c r="D114">
         <v>63.45</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114">
+        <v>574900</v>
+      </c>
+      <c r="F114">
+        <v>550891.23</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="1"/>
+        <v>24008.770000000019</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>1</v>
       </c>
@@ -2027,8 +3182,18 @@
       <c r="D115">
         <v>92.58</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <v>574999</v>
+      </c>
+      <c r="F115">
+        <v>685543.16</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="1"/>
+        <v>110544.16000000003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1</v>
       </c>
@@ -2041,8 +3206,18 @@
       <c r="D116">
         <v>73.5</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116">
+        <v>575000</v>
+      </c>
+      <c r="F116">
+        <v>610357.96</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="1"/>
+        <v>35357.959999999963</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>1</v>
       </c>
@@ -2055,8 +3230,18 @@
       <c r="D117">
         <v>76.16</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117">
+        <v>575000</v>
+      </c>
+      <c r="F117">
+        <v>620839.76</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="1"/>
+        <v>45839.760000000009</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>1</v>
       </c>
@@ -2067,10 +3252,20 @@
         <v>2</v>
       </c>
       <c r="D118">
-        <v>66.01</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66.010000000000005</v>
+      </c>
+      <c r="E118">
+        <v>575000</v>
+      </c>
+      <c r="F118">
+        <v>580843.43999999994</v>
+      </c>
+      <c r="G118">
+        <f t="shared" si="1"/>
+        <v>5843.4399999999441</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1</v>
       </c>
@@ -2083,8 +3278,18 @@
       <c r="D119">
         <v>60.88</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <v>579000</v>
+      </c>
+      <c r="F119">
+        <v>540764.07999999996</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="1"/>
+        <v>38235.920000000042</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>1</v>
       </c>
@@ -2097,8 +3302,18 @@
       <c r="D120">
         <v>55.41</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <v>579000</v>
+      </c>
+      <c r="F120">
+        <v>519209.41</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="1"/>
+        <v>59790.590000000026</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>1</v>
       </c>
@@ -2111,8 +3326,18 @@
       <c r="D121">
         <v>57.38</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <v>579000</v>
+      </c>
+      <c r="F121">
+        <v>526972.25</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="1"/>
+        <v>52027.75</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1</v>
       </c>
@@ -2125,8 +3350,18 @@
       <c r="D122">
         <v>52.94</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122">
+        <v>579000</v>
+      </c>
+      <c r="F122">
+        <v>529340.79</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="1"/>
+        <v>49659.209999999963</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>0</v>
       </c>
@@ -2137,10 +3372,20 @@
         <v>2</v>
       </c>
       <c r="D123">
-        <v>138.48</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138.47999999999999</v>
+      </c>
+      <c r="E123">
+        <v>579900</v>
+      </c>
+      <c r="F123">
+        <v>1128209.08</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="1"/>
+        <v>548309.08000000007</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>1</v>
       </c>
@@ -2153,8 +3398,18 @@
       <c r="D124">
         <v>65.95</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124">
+        <v>579900</v>
+      </c>
+      <c r="F124">
+        <v>560742.54</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="1"/>
+        <v>19157.459999999963</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>1</v>
       </c>
@@ -2167,8 +3422,18 @@
       <c r="D125">
         <v>48.33</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125">
+        <v>585000</v>
+      </c>
+      <c r="F125">
+        <v>491310.5</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="1"/>
+        <v>93689.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>1</v>
       </c>
@@ -2179,10 +3444,20 @@
         <v>2</v>
       </c>
       <c r="D126">
-        <v>68.54</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="E126">
+        <v>589000</v>
+      </c>
+      <c r="F126">
+        <v>570948.49</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="1"/>
+        <v>18051.510000000009</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>0</v>
       </c>
@@ -2195,8 +3470,18 @@
       <c r="D127">
         <v>55.39</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127">
+        <v>589000</v>
+      </c>
+      <c r="F127">
+        <v>809757.8</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="1"/>
+        <v>220757.80000000005</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>1</v>
       </c>
@@ -2207,10 +3492,20 @@
         <v>2</v>
       </c>
       <c r="D128">
-        <v>80.71</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80.709999999999994</v>
+      </c>
+      <c r="E128">
+        <v>589000</v>
+      </c>
+      <c r="F128">
+        <v>638769.14</v>
+      </c>
+      <c r="G128">
+        <f t="shared" si="1"/>
+        <v>49769.140000000014</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>1</v>
       </c>
@@ -2223,8 +3518,18 @@
       <c r="D129">
         <v>87.44</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129">
+        <v>589000</v>
+      </c>
+      <c r="F129">
+        <v>645424.4</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="1"/>
+        <v>56424.400000000023</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>1</v>
       </c>
@@ -2237,8 +3542,18 @@
       <c r="D130">
         <v>61.11</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130">
+        <v>589000</v>
+      </c>
+      <c r="F130">
+        <v>541670.40000000002</v>
+      </c>
+      <c r="G130">
+        <f t="shared" si="1"/>
+        <v>47329.599999999977</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1</v>
       </c>
@@ -2251,8 +3566,18 @@
       <c r="D131">
         <v>61.11</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131">
+        <v>589000</v>
+      </c>
+      <c r="F131">
+        <v>541670.40000000002</v>
+      </c>
+      <c r="G131">
+        <f t="shared" ref="G131:G194" si="2">ABS(E131-F131)</f>
+        <v>47329.599999999977</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>1</v>
       </c>
@@ -2265,8 +3590,18 @@
       <c r="D132">
         <v>61.98</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132">
+        <v>589000</v>
+      </c>
+      <c r="F132">
+        <v>564963.12</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="2"/>
+        <v>24036.880000000005</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>1</v>
       </c>
@@ -2279,8 +3614,18 @@
       <c r="D133">
         <v>59.88</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133">
+        <v>589800</v>
+      </c>
+      <c r="F133">
+        <v>536823.56000000006</v>
+      </c>
+      <c r="G133">
+        <f t="shared" si="2"/>
+        <v>52976.439999999944</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>1</v>
       </c>
@@ -2293,8 +3638,18 @@
       <c r="D134">
         <v>37.21</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134">
+        <v>589900</v>
+      </c>
+      <c r="F134">
+        <v>447491.87</v>
+      </c>
+      <c r="G134">
+        <f t="shared" si="2"/>
+        <v>142408.13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>1</v>
       </c>
@@ -2305,10 +3660,20 @@
         <v>2</v>
       </c>
       <c r="D135">
-        <v>37.12</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="E135">
+        <v>589900</v>
+      </c>
+      <c r="F135">
+        <v>427272.76</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="2"/>
+        <v>162627.24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>1</v>
       </c>
@@ -2321,8 +3686,18 @@
       <c r="D136">
         <v>79.2</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136">
+        <v>589900</v>
+      </c>
+      <c r="F136">
+        <v>632818.94999999995</v>
+      </c>
+      <c r="G136">
+        <f t="shared" si="2"/>
+        <v>42918.949999999953</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>1</v>
       </c>
@@ -2335,8 +3710,18 @@
       <c r="D137">
         <v>78.67</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137">
+        <v>590000</v>
+      </c>
+      <c r="F137">
+        <v>610866</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="2"/>
+        <v>20866</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>1</v>
       </c>
@@ -2349,8 +3734,18 @@
       <c r="D138">
         <v>76.11</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138">
+        <v>596500</v>
+      </c>
+      <c r="F138">
+        <v>620642.73</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="2"/>
+        <v>24142.729999999981</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>1</v>
       </c>
@@ -2363,8 +3758,18 @@
       <c r="D139">
         <v>96.03</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139">
+        <v>598900</v>
+      </c>
+      <c r="F139">
+        <v>699137.97</v>
+      </c>
+      <c r="G139">
+        <f t="shared" si="2"/>
+        <v>100237.96999999997</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>1</v>
       </c>
@@ -2377,8 +3782,18 @@
       <c r="D140">
         <v>137.62</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140">
+        <v>599000</v>
+      </c>
+      <c r="F140">
+        <v>852126.76</v>
+      </c>
+      <c r="G140">
+        <f t="shared" si="2"/>
+        <v>253126.76</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>1</v>
       </c>
@@ -2391,8 +3806,18 @@
       <c r="D141">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141">
+        <v>599000</v>
+      </c>
+      <c r="F141">
+        <v>690350.6</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="2"/>
+        <v>91350.599999999977</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>1</v>
       </c>
@@ -2405,8 +3830,18 @@
       <c r="D142">
         <v>77.09</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142">
+        <v>599000</v>
+      </c>
+      <c r="F142">
+        <v>624504.43999999994</v>
+      </c>
+      <c r="G142">
+        <f t="shared" si="2"/>
+        <v>25504.439999999944</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>1</v>
       </c>
@@ -2419,8 +3854,18 @@
       <c r="D143">
         <v>70</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <v>599000</v>
+      </c>
+      <c r="F143">
+        <v>576701.66</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="2"/>
+        <v>22298.339999999967</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>1</v>
       </c>
@@ -2433,8 +3878,18 @@
       <c r="D144">
         <v>61.11</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144">
+        <v>599000</v>
+      </c>
+      <c r="F144">
+        <v>561534.87</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="2"/>
+        <v>37465.130000000005</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>1</v>
       </c>
@@ -2447,8 +3902,18 @@
       <c r="D145">
         <v>67.25</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145">
+        <v>599000</v>
+      </c>
+      <c r="F145">
+        <v>585729.68999999994</v>
+      </c>
+      <c r="G145">
+        <f t="shared" si="2"/>
+        <v>13270.310000000056</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>1</v>
       </c>
@@ -2461,8 +3926,18 @@
       <c r="D146">
         <v>106.44</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146">
+        <v>599900</v>
+      </c>
+      <c r="F146">
+        <v>740158.83</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="2"/>
+        <v>140258.82999999996</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>1</v>
       </c>
@@ -2475,8 +3950,18 @@
       <c r="D147">
         <v>61.44</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147">
+        <v>599900</v>
+      </c>
+      <c r="F147">
+        <v>542970.77</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="2"/>
+        <v>56929.229999999981</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>1</v>
       </c>
@@ -2489,8 +3974,18 @@
       <c r="D148">
         <v>61.44</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148">
+        <v>599900</v>
+      </c>
+      <c r="F148">
+        <v>542970.77</v>
+      </c>
+      <c r="G148">
+        <f t="shared" si="2"/>
+        <v>56929.229999999981</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>1</v>
       </c>
@@ -2503,8 +3998,18 @@
       <c r="D149">
         <v>70</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149">
+        <v>599900</v>
+      </c>
+      <c r="F149">
+        <v>576701.66</v>
+      </c>
+      <c r="G149">
+        <f t="shared" si="2"/>
+        <v>23198.339999999967</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>1</v>
       </c>
@@ -2517,8 +4022,18 @@
       <c r="D150">
         <v>95.85</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150">
+        <v>599900</v>
+      </c>
+      <c r="F150">
+        <v>669597.35</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="2"/>
+        <v>69697.349999999977</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>1</v>
       </c>
@@ -2529,10 +4044,20 @@
         <v>2</v>
       </c>
       <c r="D151">
-        <v>77.21</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77.209999999999994</v>
+      </c>
+      <c r="E151">
+        <v>599900</v>
+      </c>
+      <c r="F151">
+        <v>624977.31000000006</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="2"/>
+        <v>25077.310000000056</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>1</v>
       </c>
@@ -2543,10 +4068,20 @@
         <v>2</v>
       </c>
       <c r="D152">
-        <v>74.26</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.260000000000005</v>
+      </c>
+      <c r="E152">
+        <v>599900</v>
+      </c>
+      <c r="F152">
+        <v>613352.76</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="2"/>
+        <v>13452.760000000009</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>1</v>
       </c>
@@ -2559,8 +4094,18 @@
       <c r="D153">
         <v>59.27</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153">
+        <v>599900</v>
+      </c>
+      <c r="F153">
+        <v>534419.84</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="2"/>
+        <v>65480.160000000033</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>1</v>
       </c>
@@ -2571,10 +4116,20 @@
         <v>2</v>
       </c>
       <c r="D154">
-        <v>70.79</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70.790000000000006</v>
+      </c>
+      <c r="E154">
+        <v>599900</v>
+      </c>
+      <c r="F154">
+        <v>599679.14</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="2"/>
+        <v>220.85999999998603</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>1</v>
       </c>
@@ -2587,8 +4142,18 @@
       <c r="D155">
         <v>62.27</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155">
+        <v>599999</v>
+      </c>
+      <c r="F155">
+        <v>546241.41</v>
+      </c>
+      <c r="G155">
+        <f t="shared" si="2"/>
+        <v>53757.589999999967</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>1</v>
       </c>
@@ -2601,8 +4166,18 @@
       <c r="D156">
         <v>63.08</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156">
+        <v>600000</v>
+      </c>
+      <c r="F156">
+        <v>549433.23</v>
+      </c>
+      <c r="G156">
+        <f t="shared" si="2"/>
+        <v>50566.770000000019</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>1</v>
       </c>
@@ -2615,8 +4190,18 @@
       <c r="D157">
         <v>79.23</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157">
+        <v>606000</v>
+      </c>
+      <c r="F157">
+        <v>632937.17000000004</v>
+      </c>
+      <c r="G157">
+        <f t="shared" si="2"/>
+        <v>26937.170000000042</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>1</v>
       </c>
@@ -2629,8 +4214,18 @@
       <c r="D158">
         <v>94.34</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158">
+        <v>612000</v>
+      </c>
+      <c r="F158">
+        <v>692478.48</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="2"/>
+        <v>80478.479999999981</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>1</v>
       </c>
@@ -2643,8 +4238,18 @@
       <c r="D159">
         <v>150.66</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159">
+        <v>615000</v>
+      </c>
+      <c r="F159">
+        <v>894544.33</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="2"/>
+        <v>279544.32999999996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>1</v>
       </c>
@@ -2657,8 +4262,18 @@
       <c r="D160">
         <v>88.06</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160">
+        <v>615000</v>
+      </c>
+      <c r="F160">
+        <v>647867.52</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="2"/>
+        <v>32867.520000000019</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>1</v>
       </c>
@@ -2669,10 +4284,20 @@
         <v>2</v>
       </c>
       <c r="D161">
-        <v>73.29</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73.290000000000006</v>
+      </c>
+      <c r="E161">
+        <v>619000</v>
+      </c>
+      <c r="F161">
+        <v>609530.44999999995</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="2"/>
+        <v>9469.5500000000466</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>1</v>
       </c>
@@ -2685,8 +4310,18 @@
       <c r="D162">
         <v>61.3</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162">
+        <v>619000</v>
+      </c>
+      <c r="F162">
+        <v>542419.1</v>
+      </c>
+      <c r="G162">
+        <f t="shared" si="2"/>
+        <v>76580.900000000023</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>1</v>
       </c>
@@ -2697,10 +4332,20 @@
         <v>2</v>
       </c>
       <c r="D163">
-        <v>76.51</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76.510000000000005</v>
+      </c>
+      <c r="E163">
+        <v>619900</v>
+      </c>
+      <c r="F163">
+        <v>622218.93999999994</v>
+      </c>
+      <c r="G163">
+        <f t="shared" si="2"/>
+        <v>2318.9399999999441</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>1</v>
       </c>
@@ -2711,10 +4356,20 @@
         <v>2</v>
       </c>
       <c r="D164">
-        <v>64.01</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64.010000000000005</v>
+      </c>
+      <c r="E164">
+        <v>619900</v>
+      </c>
+      <c r="F164">
+        <v>572962.39</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="2"/>
+        <v>46937.609999999986</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>1</v>
       </c>
@@ -2725,10 +4380,20 @@
         <v>2</v>
       </c>
       <c r="D165">
-        <v>64.01</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64.010000000000005</v>
+      </c>
+      <c r="E165">
+        <v>619900</v>
+      </c>
+      <c r="F165">
+        <v>572962.39</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="2"/>
+        <v>46937.609999999986</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>1</v>
       </c>
@@ -2741,8 +4406,18 @@
       <c r="D166">
         <v>74.09</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166">
+        <v>620000</v>
+      </c>
+      <c r="F166">
+        <v>592818.4</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="2"/>
+        <v>27181.599999999977</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>1</v>
       </c>
@@ -2755,8 +4430,18 @@
       <c r="D167">
         <v>154.71</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167">
+        <v>620000</v>
+      </c>
+      <c r="F167">
+        <v>930367.92</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="2"/>
+        <v>310367.92000000004</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>1</v>
       </c>
@@ -2767,10 +4452,20 @@
         <v>2</v>
       </c>
       <c r="D168">
-        <v>64.01</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64.010000000000005</v>
+      </c>
+      <c r="E168">
+        <v>625000</v>
+      </c>
+      <c r="F168">
+        <v>572962.39</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="2"/>
+        <v>52037.609999999986</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>0</v>
       </c>
@@ -2783,8 +4478,18 @@
       <c r="D169">
         <v>71.97</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169">
+        <v>629000</v>
+      </c>
+      <c r="F169">
+        <v>866124.83</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="2"/>
+        <v>237124.82999999996</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>1</v>
       </c>
@@ -2797,8 +4502,18 @@
       <c r="D170">
         <v>57.54</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170">
+        <v>629999</v>
+      </c>
+      <c r="F170">
+        <v>527602.73</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="2"/>
+        <v>102396.27000000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>1</v>
       </c>
@@ -2809,10 +4524,20 @@
         <v>2</v>
       </c>
       <c r="D171">
-        <v>73.9</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="E171">
+        <v>632000</v>
+      </c>
+      <c r="F171">
+        <v>592069.69999999995</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="2"/>
+        <v>39930.300000000047</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>1</v>
       </c>
@@ -2825,8 +4550,18 @@
       <c r="D172">
         <v>47.46</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172">
+        <v>635000</v>
+      </c>
+      <c r="F172">
+        <v>487882.25</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="2"/>
+        <v>147117.75</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>1</v>
       </c>
@@ -2839,8 +4574,18 @@
       <c r="D173">
         <v>89.45</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173">
+        <v>639000</v>
+      </c>
+      <c r="F173">
+        <v>673209.32</v>
+      </c>
+      <c r="G173">
+        <f t="shared" si="2"/>
+        <v>34209.319999999949</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>1</v>
       </c>
@@ -2853,8 +4598,18 @@
       <c r="D174">
         <v>68.52</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174">
+        <v>639999</v>
+      </c>
+      <c r="F174">
+        <v>570869.68000000005</v>
+      </c>
+      <c r="G174">
+        <f t="shared" si="2"/>
+        <v>69129.319999999949</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>1</v>
       </c>
@@ -2865,10 +4620,20 @@
         <v>2</v>
       </c>
       <c r="D175">
-        <v>67.18</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67.180000000000007</v>
+      </c>
+      <c r="E175">
+        <v>645000</v>
+      </c>
+      <c r="F175">
+        <v>585453.85</v>
+      </c>
+      <c r="G175">
+        <f t="shared" si="2"/>
+        <v>59546.150000000023</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>1</v>
       </c>
@@ -2881,8 +4646,18 @@
       <c r="D176">
         <v>82.28</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176">
+        <v>649000</v>
+      </c>
+      <c r="F176">
+        <v>644955.76</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="2"/>
+        <v>4044.2399999999907</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>1</v>
       </c>
@@ -2895,8 +4670,18 @@
       <c r="D177">
         <v>54.34</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177">
+        <v>649900</v>
+      </c>
+      <c r="F177">
+        <v>534857.52</v>
+      </c>
+      <c r="G177">
+        <f t="shared" si="2"/>
+        <v>115042.47999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>1</v>
       </c>
@@ -2909,8 +4694,18 @@
       <c r="D178">
         <v>76.02</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178">
+        <v>649900</v>
+      </c>
+      <c r="F178">
+        <v>620288.07999999996</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="2"/>
+        <v>29611.920000000042</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>1</v>
       </c>
@@ -2923,8 +4718,18 @@
       <c r="D179">
         <v>67.78</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179">
+        <v>649900</v>
+      </c>
+      <c r="F179">
+        <v>587818.16</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="2"/>
+        <v>62081.839999999967</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>1</v>
       </c>
@@ -2937,8 +4742,18 @@
       <c r="D180">
         <v>56.77</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180">
+        <v>649999</v>
+      </c>
+      <c r="F180">
+        <v>524568.53</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="2"/>
+        <v>125430.46999999997</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>1</v>
       </c>
@@ -2951,8 +4766,18 @@
       <c r="D181">
         <v>71.98</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181">
+        <v>650000</v>
+      </c>
+      <c r="F181">
+        <v>604368.37</v>
+      </c>
+      <c r="G181">
+        <f t="shared" si="2"/>
+        <v>45631.630000000005</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>1</v>
       </c>
@@ -2963,10 +4788,20 @@
         <v>2</v>
       </c>
       <c r="D182">
-        <v>67.76</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="E182">
+        <v>670000</v>
+      </c>
+      <c r="F182">
+        <v>567874.89</v>
+      </c>
+      <c r="G182">
+        <f t="shared" si="2"/>
+        <v>102125.10999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>1</v>
       </c>
@@ -2979,8 +4814,18 @@
       <c r="D183">
         <v>74.95</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183">
+        <v>673900</v>
+      </c>
+      <c r="F183">
+        <v>616071.72</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="2"/>
+        <v>57828.280000000028</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>0</v>
       </c>
@@ -2993,8 +4838,18 @@
       <c r="D184">
         <v>123.63</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184">
+        <v>674900</v>
+      </c>
+      <c r="F184">
+        <v>1087626.02</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="2"/>
+        <v>412726.02</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>1</v>
       </c>
@@ -3007,8 +4862,18 @@
       <c r="D185">
         <v>72.62</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185">
+        <v>679000</v>
+      </c>
+      <c r="F185">
+        <v>606890.30000000005</v>
+      </c>
+      <c r="G185">
+        <f t="shared" si="2"/>
+        <v>72109.699999999953</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>0</v>
       </c>
@@ -3021,8 +4886,18 @@
       <c r="D186">
         <v>83.78</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186">
+        <v>679000</v>
+      </c>
+      <c r="F186">
+        <v>950460.61</v>
+      </c>
+      <c r="G186">
+        <f t="shared" si="2"/>
+        <v>271460.61</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>1</v>
       </c>
@@ -3035,8 +4910,18 @@
       <c r="D187">
         <v>106.51</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187">
+        <v>685000</v>
+      </c>
+      <c r="F187">
+        <v>740434.66</v>
+      </c>
+      <c r="G187">
+        <f t="shared" si="2"/>
+        <v>55434.660000000033</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>0</v>
       </c>
@@ -3049,8 +4934,18 @@
       <c r="D188">
         <v>75.66</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188">
+        <v>689000</v>
+      </c>
+      <c r="F188">
+        <v>889632.22</v>
+      </c>
+      <c r="G188">
+        <f t="shared" si="2"/>
+        <v>200632.21999999997</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>1</v>
       </c>
@@ -3063,8 +4958,18 @@
       <c r="D189">
         <v>72.56</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189">
+        <v>689900</v>
+      </c>
+      <c r="F189">
+        <v>606653.87</v>
+      </c>
+      <c r="G189">
+        <f t="shared" si="2"/>
+        <v>83246.13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>1</v>
       </c>
@@ -3077,8 +4982,18 @@
       <c r="D190">
         <v>82.3</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190">
+        <v>699000</v>
+      </c>
+      <c r="F190">
+        <v>645034.56999999995</v>
+      </c>
+      <c r="G190">
+        <f t="shared" si="2"/>
+        <v>53965.430000000051</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>1</v>
       </c>
@@ -3091,8 +5006,18 @@
       <c r="D191">
         <v>87.15</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191">
+        <v>699000</v>
+      </c>
+      <c r="F191">
+        <v>664146.12</v>
+      </c>
+      <c r="G191">
+        <f t="shared" si="2"/>
+        <v>34853.880000000005</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>1</v>
       </c>
@@ -3105,8 +5030,18 @@
       <c r="D192">
         <v>75.98</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192">
+        <v>699000</v>
+      </c>
+      <c r="F192">
+        <v>620130.46</v>
+      </c>
+      <c r="G192">
+        <f t="shared" si="2"/>
+        <v>78869.540000000037</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>1</v>
       </c>
@@ -3119,8 +5054,18 @@
       <c r="D193">
         <v>55.15</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193">
+        <v>699900</v>
+      </c>
+      <c r="F193">
+        <v>518184.88</v>
+      </c>
+      <c r="G193">
+        <f t="shared" si="2"/>
+        <v>181715.12</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>0</v>
       </c>
@@ -3133,8 +5078,18 @@
       <c r="D194">
         <v>95.54</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194">
+        <v>699900</v>
+      </c>
+      <c r="F194">
+        <v>967969.84</v>
+      </c>
+      <c r="G194">
+        <f t="shared" si="2"/>
+        <v>268069.83999999997</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>1</v>
       </c>
@@ -3147,8 +5102,18 @@
       <c r="D195">
         <v>94.01</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195">
+        <v>699900</v>
+      </c>
+      <c r="F195">
+        <v>711042.58</v>
+      </c>
+      <c r="G195">
+        <f t="shared" ref="G195:G223" si="3">ABS(E195-F195)</f>
+        <v>11142.579999999958</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>1</v>
       </c>
@@ -3161,8 +5126,18 @@
       <c r="D196">
         <v>66.02</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196">
+        <v>710000</v>
+      </c>
+      <c r="F196">
+        <v>580882.84</v>
+      </c>
+      <c r="G196">
+        <f t="shared" si="3"/>
+        <v>129117.16000000003</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>1</v>
       </c>
@@ -3175,8 +5150,18 @@
       <c r="D197">
         <v>81.69</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197">
+        <v>789000</v>
+      </c>
+      <c r="F197">
+        <v>642630.85</v>
+      </c>
+      <c r="G197">
+        <f t="shared" si="3"/>
+        <v>146369.15000000002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>0</v>
       </c>
@@ -3189,8 +5174,18 @@
       <c r="D198">
         <v>98.06</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198">
+        <v>796800</v>
+      </c>
+      <c r="F198">
+        <v>997764.43</v>
+      </c>
+      <c r="G198">
+        <f t="shared" si="3"/>
+        <v>200964.43000000005</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>1</v>
       </c>
@@ -3203,8 +5198,18 @@
       <c r="D199">
         <v>77.25</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199">
+        <v>799000</v>
+      </c>
+      <c r="F199">
+        <v>605270.46</v>
+      </c>
+      <c r="G199">
+        <f t="shared" si="3"/>
+        <v>193729.54000000004</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>0</v>
       </c>
@@ -3217,8 +5222,18 @@
       <c r="D200">
         <v>119.94</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200">
+        <v>799900</v>
+      </c>
+      <c r="F200">
+        <v>1055151.77</v>
+      </c>
+      <c r="G200">
+        <f t="shared" si="3"/>
+        <v>255251.77000000002</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>0</v>
       </c>
@@ -3231,8 +5246,18 @@
       <c r="D201">
         <v>88.44</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201">
+        <v>848000</v>
+      </c>
+      <c r="F201">
+        <v>939992.12</v>
+      </c>
+      <c r="G201">
+        <f t="shared" si="3"/>
+        <v>91992.12</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>1</v>
       </c>
@@ -3245,8 +5270,18 @@
       <c r="D202">
         <v>90.88</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202">
+        <v>849999</v>
+      </c>
+      <c r="F202">
+        <v>678844.27</v>
+      </c>
+      <c r="G202">
+        <f t="shared" si="3"/>
+        <v>171154.72999999998</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>0</v>
       </c>
@@ -3259,8 +5294,18 @@
       <c r="D203">
         <v>84.35</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203">
+        <v>880000</v>
+      </c>
+      <c r="F203">
+        <v>923875.38</v>
+      </c>
+      <c r="G203">
+        <f t="shared" si="3"/>
+        <v>43875.380000000005</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>0</v>
       </c>
@@ -3271,10 +5316,20 @@
         <v>3</v>
       </c>
       <c r="D204">
-        <v>68.29</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68.290000000000006</v>
+      </c>
+      <c r="E204">
+        <v>899900</v>
+      </c>
+      <c r="F204">
+        <v>860590.56</v>
+      </c>
+      <c r="G204">
+        <f t="shared" si="3"/>
+        <v>39309.439999999944</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>0</v>
       </c>
@@ -3287,8 +5342,18 @@
       <c r="D205">
         <v>138.57</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205">
+        <v>899999</v>
+      </c>
+      <c r="F205">
+        <v>1206090.8600000001</v>
+      </c>
+      <c r="G205">
+        <f t="shared" si="3"/>
+        <v>306091.8600000001</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>0</v>
       </c>
@@ -3301,8 +5366,18 @@
       <c r="D206">
         <v>136.78</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206">
+        <v>929000</v>
+      </c>
+      <c r="F206">
+        <v>1159308.3799999999</v>
+      </c>
+      <c r="G206">
+        <f t="shared" si="3"/>
+        <v>230308.37999999989</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>0</v>
       </c>
@@ -3313,10 +5388,20 @@
         <v>3</v>
       </c>
       <c r="D207">
-        <v>131.67</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131.66999999999999</v>
+      </c>
+      <c r="E207">
+        <v>939000</v>
+      </c>
+      <c r="F207">
+        <v>1110340.98</v>
+      </c>
+      <c r="G207">
+        <f t="shared" si="3"/>
+        <v>171340.97999999998</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>1</v>
       </c>
@@ -3329,8 +5414,18 @@
       <c r="D208">
         <v>146.71</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208">
+        <v>948800</v>
+      </c>
+      <c r="F208">
+        <v>907810.59</v>
+      </c>
+      <c r="G208">
+        <f t="shared" si="3"/>
+        <v>40989.410000000033</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>0</v>
       </c>
@@ -3343,8 +5438,18 @@
       <c r="D209">
         <v>95.04</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209">
+        <v>999000</v>
+      </c>
+      <c r="F209">
+        <v>985864.05</v>
+      </c>
+      <c r="G209">
+        <f t="shared" si="3"/>
+        <v>13135.949999999953</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>0</v>
       </c>
@@ -3357,8 +5462,18 @@
       <c r="D210">
         <v>157.93</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210">
+        <v>1098000</v>
+      </c>
+      <c r="F210">
+        <v>1233683.6100000001</v>
+      </c>
+      <c r="G210">
+        <f t="shared" si="3"/>
+        <v>135683.6100000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>0</v>
       </c>
@@ -3371,8 +5486,18 @@
       <c r="D211">
         <v>134.65</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211">
+        <v>1099000</v>
+      </c>
+      <c r="F211">
+        <v>1181677.1399999999</v>
+      </c>
+      <c r="G211">
+        <f t="shared" si="3"/>
+        <v>82677.139999999898</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>0</v>
       </c>
@@ -3385,8 +5510,18 @@
       <c r="D212">
         <v>175.97</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212">
+        <v>1199900</v>
+      </c>
+      <c r="F212">
+        <v>1313737.52</v>
+      </c>
+      <c r="G212">
+        <f t="shared" si="3"/>
+        <v>113837.52000000002</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>0</v>
       </c>
@@ -3399,8 +5534,18 @@
       <c r="D213">
         <v>99.89</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213">
+        <v>1200000</v>
+      </c>
+      <c r="F213">
+        <v>1120300.9099999999</v>
+      </c>
+      <c r="G213">
+        <f t="shared" si="3"/>
+        <v>79699.090000000084</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>0</v>
       </c>
@@ -3413,8 +5558,18 @@
       <c r="D214">
         <v>226.57</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214">
+        <v>1329786</v>
+      </c>
+      <c r="F214">
+        <v>1513128.04</v>
+      </c>
+      <c r="G214">
+        <f t="shared" si="3"/>
+        <v>183342.04000000004</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>0</v>
       </c>
@@ -3427,8 +5582,18 @@
       <c r="D215">
         <v>180.86</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215">
+        <v>1349900</v>
+      </c>
+      <c r="F215">
+        <v>1333006.69</v>
+      </c>
+      <c r="G215">
+        <f t="shared" si="3"/>
+        <v>16893.310000000056</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>0</v>
       </c>
@@ -3439,10 +5604,20 @@
         <v>4</v>
       </c>
       <c r="D216">
-        <v>147.83</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147.83000000000001</v>
+      </c>
+      <c r="E216">
+        <v>1399900</v>
+      </c>
+      <c r="F216">
+        <v>1242580.1100000001</v>
+      </c>
+      <c r="G216">
+        <f t="shared" si="3"/>
+        <v>157319.8899999999</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>0</v>
       </c>
@@ -3455,8 +5630,18 @@
       <c r="D217">
         <v>196.17</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217">
+        <v>1429900</v>
+      </c>
+      <c r="F217">
+        <v>1393336.11</v>
+      </c>
+      <c r="G217">
+        <f t="shared" si="3"/>
+        <v>36563.889999999898</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>0</v>
       </c>
@@ -3469,8 +5654,18 @@
       <c r="D218">
         <v>83.78</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218">
+        <v>1499800</v>
+      </c>
+      <c r="F218">
+        <v>1001087.15</v>
+      </c>
+      <c r="G218">
+        <f t="shared" si="3"/>
+        <v>498712.85</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>1</v>
       </c>
@@ -3483,8 +5678,18 @@
       <c r="D219">
         <v>129.72</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219">
+        <v>1549990</v>
+      </c>
+      <c r="F219">
+        <v>840861.09</v>
+      </c>
+      <c r="G219">
+        <f t="shared" si="3"/>
+        <v>709128.91</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>0</v>
       </c>
@@ -3497,8 +5702,18 @@
       <c r="D220">
         <v>185.82</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220">
+        <v>1598000</v>
+      </c>
+      <c r="F220">
+        <v>1401247.48</v>
+      </c>
+      <c r="G220">
+        <f t="shared" si="3"/>
+        <v>196752.52000000002</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>0</v>
       </c>
@@ -3511,8 +5726,18 @@
       <c r="D221">
         <v>196.92</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221">
+        <v>1785800</v>
+      </c>
+      <c r="F221">
+        <v>1378357.78</v>
+      </c>
+      <c r="G221">
+        <f t="shared" si="3"/>
+        <v>407442.22</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>0</v>
       </c>
@@ -3525,8 +5750,18 @@
       <c r="D222">
         <v>62.72</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222">
+        <v>2099900</v>
+      </c>
+      <c r="F222">
+        <v>800843.65</v>
+      </c>
+      <c r="G222">
+        <f t="shared" si="3"/>
+        <v>1299056.3500000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>0</v>
       </c>
@@ -3537,11 +5772,21 @@
         <v>5</v>
       </c>
       <c r="D223">
-        <v>281.71</v>
+        <v>281.70999999999998</v>
+      </c>
+      <c r="E223">
+        <v>2988800</v>
+      </c>
+      <c r="F223">
+        <v>1759239.87</v>
+      </c>
+      <c r="G223">
+        <f t="shared" si="3"/>
+        <v>1229560.1299999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>